<commit_message>
journal de travail diogo
</commit_message>
<xml_diff>
--- a/documentation/306_Journal_travail_ArcardiaBox_DA_SILVA_DIOGO.xlsx
+++ b/documentation/306_Journal_travail_ArcardiaBox_DA_SILVA_DIOGO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-project-groupe-2\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-DaSilva\306-project-groupe-2-3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015C5A13-A282-4BAC-8F9F-82A34FDDE32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94AB351-F53D-4842-9C8C-CBF72FBFF0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Problème</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>pull des changements</t>
+  </si>
+  <si>
+    <t>installation Raspberry Pi</t>
+  </si>
+  <si>
+    <t>documentation d'installation</t>
+  </si>
+  <si>
+    <t>documentation d'utilisation</t>
+  </si>
+  <si>
+    <t>vérifier l'ergonomie</t>
+  </si>
+  <si>
+    <t>Lecture du cahier des charges</t>
+  </si>
+  <si>
+    <t>Discussion du projet</t>
   </si>
 </sst>
 </file>
@@ -257,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -447,11 +465,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -536,6 +576,50 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -544,6 +628,46 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -556,88 +680,12 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1145,11 +1193,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1166,20 +1214,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1192,13 +1240,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1208,9 +1256,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1219,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>45992</v>
       </c>
@@ -1233,15 +1281,23 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
-      <c r="B8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="C8" s="22"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
@@ -1251,7 +1307,7 @@
       </c>
       <c r="D9" s="8">
         <f>SUM(D6:D8)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,44 +1346,44 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="11">
         <f>SUM(D9,D13)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>45999</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1345,22 +1401,22 @@
       <c r="A20" s="17">
         <v>45999</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1414,10 +1470,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="10" t="s">
         <v>10</v>
       </c>
@@ -1427,15 +1483,15 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31">
+      <c r="A30" s="45">
         <v>46006</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -1448,20 +1504,20 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="7">
         <v>1</v>
       </c>
@@ -1564,10 +1620,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="10" t="s">
         <v>10</v>
       </c>
@@ -1577,26 +1633,34 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="38"/>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>45662</v>
       </c>
-      <c r="B44" s="19"/>
+      <c r="B44" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="C44" s="20"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
-      <c r="B45" s="21"/>
+      <c r="B45" s="21" t="s">
+        <v>29</v>
+      </c>
       <c r="C45" s="22"/>
-      <c r="D45" s="7"/>
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
@@ -1612,22 +1676,30 @@
       </c>
       <c r="D47" s="8">
         <f>SUM(D44:D46)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="17">
         <v>45662</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="C48" s="20"/>
-      <c r="D48" s="6"/>
+      <c r="D48" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
-      <c r="B49" s="21"/>
+      <c r="B49" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="C49" s="22"/>
-      <c r="D49" s="7"/>
+      <c r="D49" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
@@ -1643,7 +1715,7 @@
       </c>
       <c r="D51" s="8">
         <f>SUM(D48:D50)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1678,23 +1750,23 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="11">
         <f>SUM(D47,D51,D55)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="25"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="27"/>
+      <c r="A57" s="46"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="48"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
@@ -1790,10 +1862,10 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="24"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="10" t="s">
         <v>10</v>
       </c>
@@ -1808,53 +1880,24 @@
       </c>
       <c r="D72" s="9">
         <f>D14+D28+D42+D56+D70</f>
-        <v>18</v>
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A48:A51"/>
@@ -1865,19 +1908,48 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B20:C22"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D13">
     <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="Terminé">
@@ -2008,6 +2080,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100280ED870E36F6F4C976CEAC6988F82A5" ma:contentTypeVersion="37" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3169f06de23f2334ced166a676265d3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xmlns:ns3="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eab9665bb0af9cfdaba242b84d69e760" ns2:_="" ns3:_="">
     <xsd:import namespace="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
@@ -2444,15 +2525,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A574440-4762-4322-B305-C51AEF435DC1}">
   <ds:schemaRefs>
@@ -2465,6 +2537,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2481,12 +2561,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correction journal travail diogo
</commit_message>
<xml_diff>
--- a/documentation/306_Journal_travail_ArcardiaBox_DA_SILVA_DIOGO.xlsx
+++ b/documentation/306_Journal_travail_ArcardiaBox_DA_SILVA_DIOGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-DaSilva\306-project-groupe-2-3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A749EFFA-DDC4-4F73-99B3-4ABA2942F518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D32E5C2-89B9-4808-8EDC-5242C2ABBFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Problème</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>création du script d'installation automatique</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>Cette semaine j'ai principalement travaillé sur la compréhension du projet</t>
+  </si>
+  <si>
+    <t>Je pense avoir réalisé un travail utile, qui permet à d’autres personnes d’installer facilement Arcadiabox là où elles le souhaitent.</t>
   </si>
 </sst>
 </file>
@@ -278,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -420,15 +429,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -531,7 +531,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -571,6 +571,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -579,15 +587,55 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -595,7 +643,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -603,92 +651,44 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1197,10 +1197,10 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E34" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E43" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1217,20 +1217,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1243,13 +1243,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1259,9 +1259,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1284,20 +1284,20 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="7">
         <v>2</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="D9" s="8">
         <f>SUM(D6:D8)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1327,14 +1327,18 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1345,48 +1349,50 @@
       </c>
       <c r="D13" s="8">
         <f>SUM(D10:D12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="11">
         <f>SUM(D9,D13)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>45999</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1404,22 +1410,22 @@
       <c r="A20" s="17">
         <v>45999</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1447,18 +1453,18 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1473,10 +1479,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="10" t="s">
         <v>10</v>
       </c>
@@ -1486,15 +1492,15 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31">
+      <c r="A30" s="47">
         <v>46006</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -1507,20 +1513,20 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="7">
         <v>1</v>
       </c>
@@ -1550,20 +1556,20 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="7">
         <v>1</v>
       </c>
@@ -1576,7 +1582,7 @@
       </c>
       <c r="D37" s="8">
         <f>SUM(D34:D36)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1593,20 +1599,20 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="22"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="7">
         <v>1</v>
       </c>
@@ -1619,33 +1625,33 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D38:D40)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="11">
         <f>SUM(D33,D37,D41)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
-        <v>45662</v>
+        <v>46027</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>28</v>
@@ -1657,18 +1663,18 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="22"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="22"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1684,7 +1690,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="17">
-        <v>45662</v>
+        <v>46027</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>30</v>
@@ -1696,18 +1702,18 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="22"/>
+      <c r="C49" s="24"/>
       <c r="D49" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="22"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1723,7 +1729,7 @@
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17">
-        <v>45663</v>
+        <v>46028</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>29</v>
@@ -1735,18 +1741,18 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="22"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="22"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1761,10 +1767,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="10" t="s">
         <v>10</v>
       </c>
@@ -1774,29 +1780,31 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="25"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="27"/>
+      <c r="A57" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="50"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>45669</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="18"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="22"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="24"/>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="18"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="22"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1820,14 +1828,14 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="18"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="22"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="18"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="22"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1851,14 +1859,14 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="18"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="22"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="24"/>
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="18"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="22"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="24"/>
       <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1873,10 +1881,10 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="24"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="10" t="s">
         <v>10</v>
       </c>
@@ -1891,53 +1899,24 @@
       </c>
       <c r="D72" s="9">
         <f>D14+D28+D42+D56+D70</f>
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A48:A51"/>
@@ -1948,19 +1927,48 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B20:C22"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D13">
     <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="Terminé">
@@ -2091,6 +2099,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100280ED870E36F6F4C976CEAC6988F82A5" ma:contentTypeVersion="37" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3169f06de23f2334ced166a676265d3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xmlns:ns3="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eab9665bb0af9cfdaba242b84d69e760" ns2:_="" ns3:_="">
     <xsd:import namespace="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
@@ -2527,15 +2544,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A574440-4762-4322-B305-C51AEF435DC1}">
   <ds:schemaRefs>
@@ -2548,6 +2556,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2564,12 +2580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>